<commit_message>
highlighted key cells in magenta for automatic checks and added explanation of magenta
</commit_message>
<xml_diff>
--- a/honours-module-choices-SURNAME-ID-template.xlsx
+++ b/honours-module-choices-SURNAME-ID-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofstandrews907-my.sharepoint.com/personal/dwrj1_st-andrews_ac_uk/Documents/DoT/Advising/HonoursModuleChoices/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofstandrews907-my.sharepoint.com/personal/dwrj1_st-andrews_ac_uk/Documents/DoT/Advising/Advising-tool/StA_Advising/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="8_{56DABCF1-506A-CF46-B440-B9A28786DD7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{15C3A9A7-4668-334F-A252-1CA12B7C7FC8}"/>
+  <xr:revisionPtr revIDLastSave="37" documentId="8_{56DABCF1-506A-CF46-B440-B9A28786DD7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{328BC332-3E9B-474A-94D0-736751986524}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="500" windowWidth="24680" windowHeight="14900" xr2:uid="{80DCF18C-07CE-B942-AEAC-AEA347C824BB}"/>
+    <workbookView xWindow="7380" yWindow="4840" windowWidth="24680" windowHeight="21920" xr2:uid="{80DCF18C-07CE-B942-AEAC-AEA347C824BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -176,7 +176,26 @@
         <rFont val="Helvetica"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">as it will be processed (semi)automatically to ensure that your provisional choices satisfy the programme regulations. </t>
+      <t xml:space="preserve">as it will be processed (semi)automatically to ensure that your provisional choices satisfy the programme regulations. The automatic checks will read in boxes highlighted with </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t>magenta double lines</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> for any future years. </t>
     </r>
     <r>
       <rPr>
@@ -280,7 +299,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="32">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -380,21 +399,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -570,6 +574,32 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -577,7 +607,16 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -585,10 +624,8 @@
     <border>
       <left/>
       <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
+      <top/>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -598,101 +635,38 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
+      <top/>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
+      <left style="double">
+        <color rgb="FFFF40FF"/>
       </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
+      <right style="double">
+        <color rgb="FFFF40FF"/>
+      </right>
+      <top style="double">
+        <color rgb="FFFF40FF"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FFFF40FF"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -705,26 +679,62 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -732,122 +742,86 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -858,6 +832,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF40FF"/>
       <color rgb="FFF6FDF0"/>
       <color rgb="FFEFFDE7"/>
       <color rgb="FFEBF8E3"/>
@@ -875,9 +850,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -915,7 +890,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1021,7 +996,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1163,7 +1138,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1177,7 +1152,7 @@
   <dimension ref="B1:Q74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:I2"/>
+      <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="30" customHeight="1"/>
@@ -1189,66 +1164,66 @@
   <sheetData>
     <row r="1" spans="2:17" ht="11" customHeight="1" thickBot="1"/>
     <row r="2" spans="2:17" ht="120" customHeight="1" thickBot="1">
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="19"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="31"/>
     </row>
     <row r="3" spans="2:17" customFormat="1" ht="30" customHeight="1" thickBot="1"/>
-    <row r="4" spans="2:17" ht="30" customHeight="1">
-      <c r="B4" s="32" t="s">
+    <row r="4" spans="2:17" ht="30" customHeight="1" thickBot="1">
+      <c r="B4" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="33"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="21"/>
-      <c r="I4" s="22"/>
-    </row>
-    <row r="5" spans="2:17" ht="30" customHeight="1">
-      <c r="B5" s="35" t="s">
+      <c r="C4" s="36"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="39"/>
+    </row>
+    <row r="5" spans="2:17" ht="30" customHeight="1" thickTop="1" thickBot="1">
+      <c r="B5" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="36"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="24"/>
-      <c r="F5" s="24"/>
-      <c r="G5" s="24"/>
-      <c r="H5" s="24"/>
-      <c r="I5" s="25"/>
-    </row>
-    <row r="6" spans="2:17" ht="30" customHeight="1" thickBot="1">
-      <c r="B6" s="37" t="s">
+      <c r="C5" s="43"/>
+      <c r="D5" s="44"/>
+      <c r="E5" s="44"/>
+      <c r="F5" s="44"/>
+      <c r="G5" s="44"/>
+      <c r="H5" s="44"/>
+      <c r="I5" s="44"/>
+    </row>
+    <row r="6" spans="2:17" ht="30" customHeight="1" thickTop="1" thickBot="1">
+      <c r="B6" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="38"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="27"/>
-      <c r="H6" s="27"/>
-      <c r="I6" s="28"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="41"/>
+      <c r="G6" s="41"/>
+      <c r="H6" s="41"/>
+      <c r="I6" s="42"/>
     </row>
     <row r="7" spans="2:17" ht="30" customHeight="1" thickBot="1"/>
     <row r="8" spans="2:17" ht="60" customHeight="1">
-      <c r="B8" s="29" t="s">
+      <c r="B8" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="30"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="30"/>
-      <c r="G8" s="30"/>
-      <c r="H8" s="30"/>
-      <c r="I8" s="31"/>
+      <c r="C8" s="33"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="33"/>
+      <c r="H8" s="33"/>
+      <c r="I8" s="34"/>
     </row>
     <row r="9" spans="2:17" ht="30" customHeight="1" thickBot="1">
       <c r="B9" s="5"/>
@@ -1262,16 +1237,16 @@
     </row>
     <row r="10" spans="2:17" ht="30" customHeight="1" thickBot="1"/>
     <row r="11" spans="2:17" ht="59" customHeight="1">
-      <c r="B11" s="29" t="s">
+      <c r="B11" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="30"/>
-      <c r="D11" s="30"/>
-      <c r="E11" s="30"/>
-      <c r="F11" s="30"/>
-      <c r="G11" s="30"/>
-      <c r="H11" s="30"/>
-      <c r="I11" s="31"/>
+      <c r="C11" s="33"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="33"/>
+      <c r="I11" s="34"/>
       <c r="K11"/>
       <c r="L11"/>
       <c r="M11"/>
@@ -1284,19 +1259,19 @@
       <c r="B12" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="15"/>
+      <c r="C12" s="12"/>
       <c r="D12" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E12" s="15"/>
+      <c r="E12" s="12"/>
       <c r="F12" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="G12" s="15"/>
+      <c r="G12" s="12"/>
       <c r="H12" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="I12" s="16">
+      <c r="I12" s="13">
         <f>C12+E12+G12</f>
         <v>0</v>
       </c>
@@ -1318,16 +1293,16 @@
       <c r="Q13"/>
     </row>
     <row r="14" spans="2:17" ht="210" customHeight="1" thickBot="1">
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
-      <c r="H14" s="18"/>
-      <c r="I14" s="19"/>
+      <c r="C14" s="30"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="30"/>
+      <c r="H14" s="30"/>
+      <c r="I14" s="31"/>
       <c r="K14"/>
       <c r="L14"/>
       <c r="M14"/>
@@ -1346,16 +1321,16 @@
       <c r="Q15"/>
     </row>
     <row r="16" spans="2:17" ht="30" customHeight="1">
-      <c r="B16" s="39" t="s">
+      <c r="B16" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="40"/>
-      <c r="D16" s="40"/>
-      <c r="E16" s="40"/>
-      <c r="F16" s="40"/>
-      <c r="G16" s="40"/>
-      <c r="H16" s="40"/>
-      <c r="I16" s="41"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="24"/>
+      <c r="H16" s="24"/>
+      <c r="I16" s="25"/>
       <c r="K16"/>
       <c r="L16"/>
       <c r="M16"/>
@@ -1364,23 +1339,23 @@
       <c r="P16"/>
       <c r="Q16"/>
     </row>
-    <row r="17" spans="2:17" ht="30" customHeight="1">
-      <c r="B17" s="10" t="s">
+    <row r="17" spans="2:17" ht="30" customHeight="1" thickBot="1">
+      <c r="B17" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="42" t="s">
+      <c r="C17" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="D17" s="42"/>
-      <c r="E17" s="42"/>
-      <c r="F17" s="42"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="21"/>
       <c r="G17" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H17" s="42" t="s">
+      <c r="H17" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="I17" s="43"/>
+      <c r="I17" s="22"/>
       <c r="K17"/>
       <c r="L17"/>
       <c r="M17"/>
@@ -1389,15 +1364,15 @@
       <c r="P17"/>
       <c r="Q17"/>
     </row>
-    <row r="18" spans="2:17" ht="30" customHeight="1">
-      <c r="B18" s="11"/>
-      <c r="C18" s="34"/>
-      <c r="D18" s="34"/>
-      <c r="E18" s="34"/>
-      <c r="F18" s="34"/>
+    <row r="18" spans="2:17" ht="30" customHeight="1" thickTop="1" thickBot="1">
+      <c r="B18" s="48"/>
+      <c r="C18" s="45"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
       <c r="G18" s="1"/>
-      <c r="H18" s="34"/>
-      <c r="I18" s="44"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="15"/>
       <c r="K18"/>
       <c r="L18"/>
       <c r="M18"/>
@@ -1406,15 +1381,15 @@
       <c r="P18"/>
       <c r="Q18"/>
     </row>
-    <row r="19" spans="2:17" ht="30" customHeight="1">
-      <c r="B19" s="11"/>
-      <c r="C19" s="34"/>
-      <c r="D19" s="34"/>
-      <c r="E19" s="34"/>
-      <c r="F19" s="34"/>
+    <row r="19" spans="2:17" ht="30" customHeight="1" thickTop="1" thickBot="1">
+      <c r="B19" s="48"/>
+      <c r="C19" s="45"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
       <c r="G19" s="1"/>
-      <c r="H19" s="34"/>
-      <c r="I19" s="44"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="15"/>
       <c r="K19"/>
       <c r="L19"/>
       <c r="M19"/>
@@ -1423,15 +1398,15 @@
       <c r="P19"/>
       <c r="Q19"/>
     </row>
-    <row r="20" spans="2:17" ht="30" customHeight="1">
-      <c r="B20" s="11"/>
-      <c r="C20" s="34"/>
-      <c r="D20" s="34"/>
-      <c r="E20" s="34"/>
-      <c r="F20" s="34"/>
+    <row r="20" spans="2:17" ht="30" customHeight="1" thickTop="1" thickBot="1">
+      <c r="B20" s="48"/>
+      <c r="C20" s="45"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
       <c r="G20" s="1"/>
-      <c r="H20" s="34"/>
-      <c r="I20" s="44"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="15"/>
       <c r="K20"/>
       <c r="L20"/>
       <c r="M20"/>
@@ -1440,15 +1415,15 @@
       <c r="P20"/>
       <c r="Q20"/>
     </row>
-    <row r="21" spans="2:17" ht="30" customHeight="1">
-      <c r="B21" s="11"/>
-      <c r="C21" s="34"/>
-      <c r="D21" s="34"/>
-      <c r="E21" s="34"/>
-      <c r="F21" s="34"/>
+    <row r="21" spans="2:17" ht="30" customHeight="1" thickTop="1" thickBot="1">
+      <c r="B21" s="48"/>
+      <c r="C21" s="45"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
       <c r="G21" s="1"/>
-      <c r="H21" s="34"/>
-      <c r="I21" s="44"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="15"/>
       <c r="K21"/>
       <c r="L21"/>
       <c r="M21"/>
@@ -1457,15 +1432,15 @@
       <c r="P21"/>
       <c r="Q21"/>
     </row>
-    <row r="22" spans="2:17" ht="30" customHeight="1">
-      <c r="B22" s="11"/>
-      <c r="C22" s="34"/>
-      <c r="D22" s="34"/>
-      <c r="E22" s="34"/>
-      <c r="F22" s="34"/>
+    <row r="22" spans="2:17" ht="30" customHeight="1" thickTop="1" thickBot="1">
+      <c r="B22" s="48"/>
+      <c r="C22" s="45"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
       <c r="G22" s="1"/>
-      <c r="H22" s="34"/>
-      <c r="I22" s="44"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="15"/>
       <c r="K22"/>
       <c r="L22"/>
       <c r="M22"/>
@@ -1474,15 +1449,15 @@
       <c r="P22"/>
       <c r="Q22"/>
     </row>
-    <row r="23" spans="2:17" ht="30" customHeight="1" thickBot="1">
-      <c r="B23" s="5"/>
-      <c r="C23" s="45"/>
-      <c r="D23" s="45"/>
-      <c r="E23" s="45"/>
-      <c r="F23" s="45"/>
+    <row r="23" spans="2:17" ht="30" customHeight="1" thickTop="1" thickBot="1">
+      <c r="B23" s="48"/>
+      <c r="C23" s="46"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="16"/>
       <c r="G23" s="2"/>
-      <c r="H23" s="45"/>
-      <c r="I23" s="46"/>
+      <c r="H23" s="16"/>
+      <c r="I23" s="17"/>
       <c r="K23"/>
       <c r="L23"/>
       <c r="M23"/>
@@ -1491,11 +1466,11 @@
       <c r="P23"/>
       <c r="Q23"/>
     </row>
-    <row r="24" spans="2:17" ht="30" customHeight="1" thickBot="1">
-      <c r="F24" s="13" t="s">
+    <row r="24" spans="2:17" ht="30" customHeight="1" thickTop="1" thickBot="1">
+      <c r="F24" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="G24" s="12">
+      <c r="G24" s="10">
         <f>SUM(G18:G23)</f>
         <v>0</v>
       </c>
@@ -1517,16 +1492,16 @@
       <c r="Q25"/>
     </row>
     <row r="26" spans="2:17" ht="30" customHeight="1">
-      <c r="B26" s="39" t="s">
+      <c r="B26" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="C26" s="40"/>
-      <c r="D26" s="40"/>
-      <c r="E26" s="40"/>
-      <c r="F26" s="40"/>
-      <c r="G26" s="40"/>
-      <c r="H26" s="40"/>
-      <c r="I26" s="41"/>
+      <c r="C26" s="24"/>
+      <c r="D26" s="24"/>
+      <c r="E26" s="24"/>
+      <c r="F26" s="24"/>
+      <c r="G26" s="24"/>
+      <c r="H26" s="24"/>
+      <c r="I26" s="25"/>
       <c r="K26"/>
       <c r="L26"/>
       <c r="M26"/>
@@ -1535,23 +1510,23 @@
       <c r="P26"/>
       <c r="Q26"/>
     </row>
-    <row r="27" spans="2:17" ht="30" customHeight="1">
-      <c r="B27" s="10" t="s">
+    <row r="27" spans="2:17" ht="30" customHeight="1" thickBot="1">
+      <c r="B27" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="C27" s="42" t="s">
+      <c r="C27" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="D27" s="42"/>
-      <c r="E27" s="42"/>
-      <c r="F27" s="42"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="21"/>
       <c r="G27" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H27" s="42" t="s">
+      <c r="H27" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="I27" s="43"/>
+      <c r="I27" s="22"/>
       <c r="K27"/>
       <c r="L27"/>
       <c r="M27"/>
@@ -1560,15 +1535,15 @@
       <c r="P27"/>
       <c r="Q27"/>
     </row>
-    <row r="28" spans="2:17" ht="30" customHeight="1">
-      <c r="B28" s="11"/>
-      <c r="C28" s="34"/>
-      <c r="D28" s="34"/>
-      <c r="E28" s="34"/>
-      <c r="F28" s="34"/>
+    <row r="28" spans="2:17" ht="30" customHeight="1" thickTop="1" thickBot="1">
+      <c r="B28" s="48"/>
+      <c r="C28" s="45"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="14"/>
       <c r="G28" s="1"/>
-      <c r="H28" s="34"/>
-      <c r="I28" s="44"/>
+      <c r="H28" s="14"/>
+      <c r="I28" s="15"/>
       <c r="K28"/>
       <c r="L28"/>
       <c r="M28"/>
@@ -1577,15 +1552,15 @@
       <c r="P28"/>
       <c r="Q28"/>
     </row>
-    <row r="29" spans="2:17" ht="30" customHeight="1">
-      <c r="B29" s="11"/>
-      <c r="C29" s="34"/>
-      <c r="D29" s="34"/>
-      <c r="E29" s="34"/>
-      <c r="F29" s="34"/>
+    <row r="29" spans="2:17" ht="30" customHeight="1" thickTop="1" thickBot="1">
+      <c r="B29" s="48"/>
+      <c r="C29" s="45"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="14"/>
       <c r="G29" s="1"/>
-      <c r="H29" s="34"/>
-      <c r="I29" s="44"/>
+      <c r="H29" s="14"/>
+      <c r="I29" s="15"/>
       <c r="K29"/>
       <c r="L29"/>
       <c r="M29"/>
@@ -1594,15 +1569,15 @@
       <c r="P29"/>
       <c r="Q29"/>
     </row>
-    <row r="30" spans="2:17" ht="30" customHeight="1">
-      <c r="B30" s="11"/>
-      <c r="C30" s="34"/>
-      <c r="D30" s="34"/>
-      <c r="E30" s="34"/>
-      <c r="F30" s="34"/>
+    <row r="30" spans="2:17" ht="30" customHeight="1" thickTop="1" thickBot="1">
+      <c r="B30" s="48"/>
+      <c r="C30" s="45"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="14"/>
+      <c r="F30" s="14"/>
       <c r="G30" s="1"/>
-      <c r="H30" s="34"/>
-      <c r="I30" s="44"/>
+      <c r="H30" s="14"/>
+      <c r="I30" s="15"/>
       <c r="K30"/>
       <c r="L30"/>
       <c r="M30"/>
@@ -1611,15 +1586,15 @@
       <c r="P30"/>
       <c r="Q30"/>
     </row>
-    <row r="31" spans="2:17" ht="30" customHeight="1">
-      <c r="B31" s="11"/>
-      <c r="C31" s="34"/>
-      <c r="D31" s="34"/>
-      <c r="E31" s="34"/>
-      <c r="F31" s="34"/>
+    <row r="31" spans="2:17" ht="30" customHeight="1" thickTop="1" thickBot="1">
+      <c r="B31" s="48"/>
+      <c r="C31" s="45"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="14"/>
+      <c r="F31" s="14"/>
       <c r="G31" s="1"/>
-      <c r="H31" s="34"/>
-      <c r="I31" s="44"/>
+      <c r="H31" s="14"/>
+      <c r="I31" s="15"/>
       <c r="K31"/>
       <c r="L31"/>
       <c r="M31"/>
@@ -1628,15 +1603,15 @@
       <c r="P31"/>
       <c r="Q31"/>
     </row>
-    <row r="32" spans="2:17" ht="30" customHeight="1">
-      <c r="B32" s="11"/>
-      <c r="C32" s="34"/>
-      <c r="D32" s="34"/>
-      <c r="E32" s="34"/>
-      <c r="F32" s="34"/>
+    <row r="32" spans="2:17" ht="30" customHeight="1" thickTop="1" thickBot="1">
+      <c r="B32" s="48"/>
+      <c r="C32" s="45"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="14"/>
+      <c r="F32" s="14"/>
       <c r="G32" s="1"/>
-      <c r="H32" s="34"/>
-      <c r="I32" s="44"/>
+      <c r="H32" s="14"/>
+      <c r="I32" s="15"/>
       <c r="K32"/>
       <c r="L32"/>
       <c r="M32"/>
@@ -1645,15 +1620,15 @@
       <c r="P32"/>
       <c r="Q32"/>
     </row>
-    <row r="33" spans="2:17" ht="30" customHeight="1" thickBot="1">
-      <c r="B33" s="5"/>
-      <c r="C33" s="45"/>
-      <c r="D33" s="45"/>
-      <c r="E33" s="45"/>
-      <c r="F33" s="45"/>
+    <row r="33" spans="2:17" ht="30" customHeight="1" thickTop="1" thickBot="1">
+      <c r="B33" s="48"/>
+      <c r="C33" s="46"/>
+      <c r="D33" s="16"/>
+      <c r="E33" s="16"/>
+      <c r="F33" s="16"/>
       <c r="G33" s="2"/>
-      <c r="H33" s="45"/>
-      <c r="I33" s="46"/>
+      <c r="H33" s="16"/>
+      <c r="I33" s="17"/>
       <c r="K33"/>
       <c r="L33"/>
       <c r="M33"/>
@@ -1662,11 +1637,11 @@
       <c r="P33"/>
       <c r="Q33"/>
     </row>
-    <row r="34" spans="2:17" ht="30" customHeight="1" thickBot="1">
-      <c r="F34" s="13" t="s">
+    <row r="34" spans="2:17" ht="30" customHeight="1" thickTop="1" thickBot="1">
+      <c r="F34" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="G34" s="12">
+      <c r="G34" s="10">
         <f>SUM(G28:G33)</f>
         <v>0</v>
       </c>
@@ -1688,16 +1663,16 @@
       <c r="Q35"/>
     </row>
     <row r="36" spans="2:17" ht="30" customHeight="1">
-      <c r="B36" s="39" t="s">
+      <c r="B36" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="C36" s="40"/>
-      <c r="D36" s="40"/>
-      <c r="E36" s="40"/>
-      <c r="F36" s="40"/>
-      <c r="G36" s="40"/>
-      <c r="H36" s="40"/>
-      <c r="I36" s="41"/>
+      <c r="C36" s="24"/>
+      <c r="D36" s="24"/>
+      <c r="E36" s="24"/>
+      <c r="F36" s="24"/>
+      <c r="G36" s="24"/>
+      <c r="H36" s="24"/>
+      <c r="I36" s="25"/>
       <c r="K36"/>
       <c r="L36"/>
       <c r="M36"/>
@@ -1706,23 +1681,23 @@
       <c r="P36"/>
       <c r="Q36"/>
     </row>
-    <row r="37" spans="2:17" ht="30" customHeight="1">
-      <c r="B37" s="10" t="s">
+    <row r="37" spans="2:17" ht="30" customHeight="1" thickBot="1">
+      <c r="B37" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="C37" s="42" t="s">
+      <c r="C37" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="D37" s="42"/>
-      <c r="E37" s="42"/>
-      <c r="F37" s="42"/>
+      <c r="D37" s="21"/>
+      <c r="E37" s="21"/>
+      <c r="F37" s="21"/>
       <c r="G37" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H37" s="42" t="s">
+      <c r="H37" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="I37" s="43"/>
+      <c r="I37" s="22"/>
       <c r="K37"/>
       <c r="L37"/>
       <c r="M37"/>
@@ -1731,15 +1706,15 @@
       <c r="P37"/>
       <c r="Q37"/>
     </row>
-    <row r="38" spans="2:17" ht="30" customHeight="1">
-      <c r="B38" s="11"/>
-      <c r="C38" s="34"/>
-      <c r="D38" s="34"/>
-      <c r="E38" s="34"/>
-      <c r="F38" s="34"/>
+    <row r="38" spans="2:17" ht="30" customHeight="1" thickTop="1" thickBot="1">
+      <c r="B38" s="48"/>
+      <c r="C38" s="45"/>
+      <c r="D38" s="14"/>
+      <c r="E38" s="14"/>
+      <c r="F38" s="14"/>
       <c r="G38" s="1"/>
-      <c r="H38" s="34"/>
-      <c r="I38" s="44"/>
+      <c r="H38" s="14"/>
+      <c r="I38" s="15"/>
       <c r="K38"/>
       <c r="L38"/>
       <c r="M38"/>
@@ -1748,15 +1723,15 @@
       <c r="P38"/>
       <c r="Q38"/>
     </row>
-    <row r="39" spans="2:17" ht="30" customHeight="1">
-      <c r="B39" s="11"/>
-      <c r="C39" s="34"/>
-      <c r="D39" s="34"/>
-      <c r="E39" s="34"/>
-      <c r="F39" s="34"/>
+    <row r="39" spans="2:17" ht="30" customHeight="1" thickTop="1" thickBot="1">
+      <c r="B39" s="48"/>
+      <c r="C39" s="45"/>
+      <c r="D39" s="14"/>
+      <c r="E39" s="14"/>
+      <c r="F39" s="14"/>
       <c r="G39" s="1"/>
-      <c r="H39" s="34"/>
-      <c r="I39" s="44"/>
+      <c r="H39" s="14"/>
+      <c r="I39" s="15"/>
       <c r="K39"/>
       <c r="L39"/>
       <c r="M39"/>
@@ -1765,15 +1740,15 @@
       <c r="P39"/>
       <c r="Q39"/>
     </row>
-    <row r="40" spans="2:17" ht="30" customHeight="1">
-      <c r="B40" s="11"/>
-      <c r="C40" s="34"/>
-      <c r="D40" s="34"/>
-      <c r="E40" s="34"/>
-      <c r="F40" s="34"/>
+    <row r="40" spans="2:17" ht="30" customHeight="1" thickTop="1" thickBot="1">
+      <c r="B40" s="48"/>
+      <c r="C40" s="45"/>
+      <c r="D40" s="14"/>
+      <c r="E40" s="14"/>
+      <c r="F40" s="14"/>
       <c r="G40" s="1"/>
-      <c r="H40" s="34"/>
-      <c r="I40" s="44"/>
+      <c r="H40" s="14"/>
+      <c r="I40" s="15"/>
       <c r="K40"/>
       <c r="L40"/>
       <c r="M40"/>
@@ -1782,15 +1757,15 @@
       <c r="P40"/>
       <c r="Q40"/>
     </row>
-    <row r="41" spans="2:17" ht="30" customHeight="1">
-      <c r="B41" s="11"/>
-      <c r="C41" s="34"/>
-      <c r="D41" s="34"/>
-      <c r="E41" s="34"/>
-      <c r="F41" s="34"/>
+    <row r="41" spans="2:17" ht="30" customHeight="1" thickTop="1" thickBot="1">
+      <c r="B41" s="48"/>
+      <c r="C41" s="45"/>
+      <c r="D41" s="14"/>
+      <c r="E41" s="14"/>
+      <c r="F41" s="14"/>
       <c r="G41" s="1"/>
-      <c r="H41" s="34"/>
-      <c r="I41" s="44"/>
+      <c r="H41" s="14"/>
+      <c r="I41" s="15"/>
       <c r="K41"/>
       <c r="L41"/>
       <c r="M41"/>
@@ -1799,15 +1774,15 @@
       <c r="P41"/>
       <c r="Q41"/>
     </row>
-    <row r="42" spans="2:17" ht="30" customHeight="1">
-      <c r="B42" s="11"/>
-      <c r="C42" s="34"/>
-      <c r="D42" s="34"/>
-      <c r="E42" s="34"/>
-      <c r="F42" s="34"/>
+    <row r="42" spans="2:17" ht="30" customHeight="1" thickTop="1" thickBot="1">
+      <c r="B42" s="48"/>
+      <c r="C42" s="45"/>
+      <c r="D42" s="14"/>
+      <c r="E42" s="14"/>
+      <c r="F42" s="14"/>
       <c r="G42" s="1"/>
-      <c r="H42" s="34"/>
-      <c r="I42" s="44"/>
+      <c r="H42" s="14"/>
+      <c r="I42" s="15"/>
       <c r="K42"/>
       <c r="L42"/>
       <c r="M42"/>
@@ -1816,15 +1791,15 @@
       <c r="P42"/>
       <c r="Q42"/>
     </row>
-    <row r="43" spans="2:17" ht="30" customHeight="1" thickBot="1">
-      <c r="B43" s="5"/>
-      <c r="C43" s="45"/>
-      <c r="D43" s="45"/>
-      <c r="E43" s="45"/>
-      <c r="F43" s="45"/>
+    <row r="43" spans="2:17" ht="30" customHeight="1" thickTop="1" thickBot="1">
+      <c r="B43" s="48"/>
+      <c r="C43" s="46"/>
+      <c r="D43" s="16"/>
+      <c r="E43" s="16"/>
+      <c r="F43" s="16"/>
       <c r="G43" s="2"/>
-      <c r="H43" s="45"/>
-      <c r="I43" s="46"/>
+      <c r="H43" s="16"/>
+      <c r="I43" s="17"/>
       <c r="K43"/>
       <c r="L43"/>
       <c r="M43"/>
@@ -1833,11 +1808,11 @@
       <c r="P43"/>
       <c r="Q43"/>
     </row>
-    <row r="44" spans="2:17" ht="30" customHeight="1" thickBot="1">
-      <c r="F44" s="13" t="s">
+    <row r="44" spans="2:17" ht="30" customHeight="1" thickTop="1" thickBot="1">
+      <c r="F44" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="G44" s="12">
+      <c r="G44" s="10">
         <f>SUM(G38:G43)</f>
         <v>0</v>
       </c>
@@ -1859,16 +1834,16 @@
       <c r="Q45"/>
     </row>
     <row r="46" spans="2:17" ht="60" customHeight="1">
-      <c r="B46" s="47" t="s">
+      <c r="B46" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="C46" s="48"/>
-      <c r="D46" s="48"/>
-      <c r="E46" s="48"/>
-      <c r="F46" s="48"/>
-      <c r="G46" s="48"/>
-      <c r="H46" s="48"/>
-      <c r="I46" s="49"/>
+      <c r="C46" s="19"/>
+      <c r="D46" s="19"/>
+      <c r="E46" s="19"/>
+      <c r="F46" s="19"/>
+      <c r="G46" s="19"/>
+      <c r="H46" s="19"/>
+      <c r="I46" s="20"/>
       <c r="K46"/>
       <c r="L46"/>
       <c r="M46"/>
@@ -1877,23 +1852,23 @@
       <c r="P46"/>
       <c r="Q46"/>
     </row>
-    <row r="47" spans="2:17" ht="30" customHeight="1">
-      <c r="B47" s="14" t="s">
+    <row r="47" spans="2:17" ht="30" customHeight="1" thickBot="1">
+      <c r="B47" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="C47" s="42" t="s">
+      <c r="C47" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="D47" s="42"/>
-      <c r="E47" s="42"/>
-      <c r="F47" s="42"/>
+      <c r="D47" s="21"/>
+      <c r="E47" s="21"/>
+      <c r="F47" s="21"/>
       <c r="G47" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H47" s="42" t="s">
+      <c r="H47" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="I47" s="43"/>
+      <c r="I47" s="22"/>
       <c r="K47"/>
       <c r="L47"/>
       <c r="M47"/>
@@ -1902,15 +1877,15 @@
       <c r="P47"/>
       <c r="Q47"/>
     </row>
-    <row r="48" spans="2:17" ht="30" customHeight="1">
-      <c r="B48" s="11"/>
-      <c r="C48" s="34"/>
-      <c r="D48" s="34"/>
-      <c r="E48" s="34"/>
-      <c r="F48" s="34"/>
+    <row r="48" spans="2:17" ht="30" customHeight="1" thickTop="1" thickBot="1">
+      <c r="B48" s="48"/>
+      <c r="C48" s="45"/>
+      <c r="D48" s="14"/>
+      <c r="E48" s="14"/>
+      <c r="F48" s="14"/>
       <c r="G48" s="1"/>
-      <c r="H48" s="34"/>
-      <c r="I48" s="44"/>
+      <c r="H48" s="14"/>
+      <c r="I48" s="15"/>
       <c r="K48"/>
       <c r="L48"/>
       <c r="M48"/>
@@ -1919,15 +1894,15 @@
       <c r="P48"/>
       <c r="Q48"/>
     </row>
-    <row r="49" spans="2:17" ht="30" customHeight="1">
-      <c r="B49" s="11"/>
-      <c r="C49" s="34"/>
-      <c r="D49" s="34"/>
-      <c r="E49" s="34"/>
-      <c r="F49" s="34"/>
+    <row r="49" spans="2:17" ht="30" customHeight="1" thickTop="1" thickBot="1">
+      <c r="B49" s="48"/>
+      <c r="C49" s="45"/>
+      <c r="D49" s="14"/>
+      <c r="E49" s="14"/>
+      <c r="F49" s="14"/>
       <c r="G49" s="1"/>
-      <c r="H49" s="34"/>
-      <c r="I49" s="44"/>
+      <c r="H49" s="14"/>
+      <c r="I49" s="15"/>
       <c r="K49"/>
       <c r="L49"/>
       <c r="M49"/>
@@ -1936,15 +1911,15 @@
       <c r="P49"/>
       <c r="Q49"/>
     </row>
-    <row r="50" spans="2:17" ht="30" customHeight="1">
-      <c r="B50" s="11"/>
-      <c r="C50" s="34"/>
-      <c r="D50" s="34"/>
-      <c r="E50" s="34"/>
-      <c r="F50" s="34"/>
+    <row r="50" spans="2:17" ht="30" customHeight="1" thickTop="1" thickBot="1">
+      <c r="B50" s="48"/>
+      <c r="C50" s="45"/>
+      <c r="D50" s="14"/>
+      <c r="E50" s="14"/>
+      <c r="F50" s="14"/>
       <c r="G50" s="1"/>
-      <c r="H50" s="34"/>
-      <c r="I50" s="44"/>
+      <c r="H50" s="14"/>
+      <c r="I50" s="15"/>
       <c r="K50"/>
       <c r="L50"/>
       <c r="M50"/>
@@ -1953,15 +1928,15 @@
       <c r="P50"/>
       <c r="Q50"/>
     </row>
-    <row r="51" spans="2:17" ht="30" customHeight="1">
-      <c r="B51" s="11"/>
-      <c r="C51" s="34"/>
-      <c r="D51" s="34"/>
-      <c r="E51" s="34"/>
-      <c r="F51" s="34"/>
+    <row r="51" spans="2:17" ht="30" customHeight="1" thickTop="1" thickBot="1">
+      <c r="B51" s="48"/>
+      <c r="C51" s="45"/>
+      <c r="D51" s="14"/>
+      <c r="E51" s="14"/>
+      <c r="F51" s="14"/>
       <c r="G51" s="1"/>
-      <c r="H51" s="34"/>
-      <c r="I51" s="44"/>
+      <c r="H51" s="14"/>
+      <c r="I51" s="15"/>
       <c r="K51"/>
       <c r="L51"/>
       <c r="M51"/>
@@ -1970,15 +1945,15 @@
       <c r="P51"/>
       <c r="Q51"/>
     </row>
-    <row r="52" spans="2:17" ht="30" customHeight="1">
-      <c r="B52" s="11"/>
-      <c r="C52" s="34"/>
-      <c r="D52" s="34"/>
-      <c r="E52" s="34"/>
-      <c r="F52" s="34"/>
+    <row r="52" spans="2:17" ht="30" customHeight="1" thickTop="1" thickBot="1">
+      <c r="B52" s="48"/>
+      <c r="C52" s="45"/>
+      <c r="D52" s="14"/>
+      <c r="E52" s="14"/>
+      <c r="F52" s="14"/>
       <c r="G52" s="1"/>
-      <c r="H52" s="34"/>
-      <c r="I52" s="44"/>
+      <c r="H52" s="14"/>
+      <c r="I52" s="15"/>
       <c r="K52"/>
       <c r="L52"/>
       <c r="M52"/>
@@ -1987,237 +1962,304 @@
       <c r="P52"/>
       <c r="Q52"/>
     </row>
-    <row r="53" spans="2:17" ht="30" customHeight="1" thickBot="1">
-      <c r="B53" s="5"/>
-      <c r="C53" s="45"/>
-      <c r="D53" s="45"/>
-      <c r="E53" s="45"/>
-      <c r="F53" s="45"/>
+    <row r="53" spans="2:17" ht="30" customHeight="1" thickTop="1" thickBot="1">
+      <c r="B53" s="48"/>
+      <c r="C53" s="46"/>
+      <c r="D53" s="16"/>
+      <c r="E53" s="16"/>
+      <c r="F53" s="16"/>
       <c r="G53" s="2"/>
-      <c r="H53" s="45"/>
-      <c r="I53" s="46"/>
-    </row>
-    <row r="54" spans="2:17" ht="30" customHeight="1" thickBot="1">
-      <c r="F54" s="13" t="s">
+      <c r="H53" s="16"/>
+      <c r="I53" s="17"/>
+    </row>
+    <row r="54" spans="2:17" ht="30" customHeight="1" thickTop="1" thickBot="1">
+      <c r="F54" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="G54" s="12">
+      <c r="G54" s="10">
         <f>SUM(G48:G53)</f>
         <v>0</v>
       </c>
     </row>
     <row r="55" spans="2:17" ht="30" customHeight="1" thickBot="1"/>
     <row r="56" spans="2:17" ht="30" customHeight="1">
-      <c r="B56" s="39" t="s">
+      <c r="B56" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="C56" s="40"/>
-      <c r="D56" s="40"/>
-      <c r="E56" s="40"/>
-      <c r="F56" s="40"/>
-      <c r="G56" s="40"/>
-      <c r="H56" s="40"/>
-      <c r="I56" s="41"/>
-    </row>
-    <row r="57" spans="2:17" ht="30" customHeight="1">
-      <c r="B57" s="10" t="s">
+      <c r="C56" s="24"/>
+      <c r="D56" s="24"/>
+      <c r="E56" s="24"/>
+      <c r="F56" s="24"/>
+      <c r="G56" s="24"/>
+      <c r="H56" s="24"/>
+      <c r="I56" s="25"/>
+    </row>
+    <row r="57" spans="2:17" ht="30" customHeight="1" thickBot="1">
+      <c r="B57" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="C57" s="42" t="s">
+      <c r="C57" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="D57" s="42"/>
-      <c r="E57" s="42"/>
-      <c r="F57" s="42"/>
+      <c r="D57" s="21"/>
+      <c r="E57" s="21"/>
+      <c r="F57" s="21"/>
       <c r="G57" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H57" s="42" t="s">
+      <c r="H57" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="I57" s="43"/>
-    </row>
-    <row r="58" spans="2:17" ht="30" customHeight="1">
-      <c r="B58" s="11"/>
-      <c r="C58" s="34"/>
-      <c r="D58" s="34"/>
-      <c r="E58" s="34"/>
-      <c r="F58" s="34"/>
+      <c r="I57" s="22"/>
+    </row>
+    <row r="58" spans="2:17" ht="30" customHeight="1" thickTop="1" thickBot="1">
+      <c r="B58" s="48"/>
+      <c r="C58" s="45"/>
+      <c r="D58" s="14"/>
+      <c r="E58" s="14"/>
+      <c r="F58" s="14"/>
       <c r="G58" s="1"/>
-      <c r="H58" s="34"/>
-      <c r="I58" s="44"/>
-    </row>
-    <row r="59" spans="2:17" ht="30" customHeight="1">
-      <c r="B59" s="11"/>
-      <c r="C59" s="34"/>
-      <c r="D59" s="34"/>
-      <c r="E59" s="34"/>
-      <c r="F59" s="34"/>
+      <c r="H58" s="14"/>
+      <c r="I58" s="15"/>
+    </row>
+    <row r="59" spans="2:17" ht="30" customHeight="1" thickTop="1" thickBot="1">
+      <c r="B59" s="48"/>
+      <c r="C59" s="45"/>
+      <c r="D59" s="14"/>
+      <c r="E59" s="14"/>
+      <c r="F59" s="14"/>
       <c r="G59" s="1"/>
-      <c r="H59" s="34"/>
-      <c r="I59" s="44"/>
-    </row>
-    <row r="60" spans="2:17" ht="30" customHeight="1">
-      <c r="B60" s="11"/>
-      <c r="C60" s="34"/>
-      <c r="D60" s="34"/>
-      <c r="E60" s="34"/>
-      <c r="F60" s="34"/>
+      <c r="H59" s="14"/>
+      <c r="I59" s="15"/>
+    </row>
+    <row r="60" spans="2:17" ht="30" customHeight="1" thickTop="1" thickBot="1">
+      <c r="B60" s="48"/>
+      <c r="C60" s="45"/>
+      <c r="D60" s="14"/>
+      <c r="E60" s="14"/>
+      <c r="F60" s="14"/>
       <c r="G60" s="1"/>
-      <c r="H60" s="34"/>
-      <c r="I60" s="44"/>
-    </row>
-    <row r="61" spans="2:17" ht="30" customHeight="1">
-      <c r="B61" s="11"/>
-      <c r="C61" s="34"/>
-      <c r="D61" s="34"/>
-      <c r="E61" s="34"/>
-      <c r="F61" s="34"/>
+      <c r="H60" s="14"/>
+      <c r="I60" s="15"/>
+    </row>
+    <row r="61" spans="2:17" ht="30" customHeight="1" thickTop="1" thickBot="1">
+      <c r="B61" s="48"/>
+      <c r="C61" s="45"/>
+      <c r="D61" s="14"/>
+      <c r="E61" s="14"/>
+      <c r="F61" s="14"/>
       <c r="G61" s="1"/>
-      <c r="H61" s="34"/>
-      <c r="I61" s="44"/>
-    </row>
-    <row r="62" spans="2:17" ht="30" customHeight="1">
-      <c r="B62" s="11"/>
-      <c r="C62" s="34"/>
-      <c r="D62" s="34"/>
-      <c r="E62" s="34"/>
-      <c r="F62" s="34"/>
+      <c r="H61" s="14"/>
+      <c r="I61" s="15"/>
+    </row>
+    <row r="62" spans="2:17" ht="30" customHeight="1" thickTop="1" thickBot="1">
+      <c r="B62" s="48"/>
+      <c r="C62" s="45"/>
+      <c r="D62" s="14"/>
+      <c r="E62" s="14"/>
+      <c r="F62" s="14"/>
       <c r="G62" s="1"/>
-      <c r="H62" s="34"/>
-      <c r="I62" s="44"/>
-    </row>
-    <row r="63" spans="2:17" ht="30" customHeight="1" thickBot="1">
-      <c r="B63" s="5"/>
-      <c r="C63" s="45"/>
-      <c r="D63" s="45"/>
-      <c r="E63" s="45"/>
-      <c r="F63" s="45"/>
+      <c r="H62" s="14"/>
+      <c r="I62" s="15"/>
+    </row>
+    <row r="63" spans="2:17" ht="30" customHeight="1" thickTop="1" thickBot="1">
+      <c r="B63" s="48"/>
+      <c r="C63" s="46"/>
+      <c r="D63" s="16"/>
+      <c r="E63" s="16"/>
+      <c r="F63" s="16"/>
       <c r="G63" s="2"/>
-      <c r="H63" s="45"/>
-      <c r="I63" s="46"/>
-    </row>
-    <row r="64" spans="2:17" ht="30" customHeight="1" thickBot="1">
-      <c r="F64" s="13" t="s">
+      <c r="H63" s="16"/>
+      <c r="I63" s="17"/>
+    </row>
+    <row r="64" spans="2:17" ht="30" customHeight="1" thickTop="1" thickBot="1">
+      <c r="F64" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="G64" s="12">
+      <c r="G64" s="10">
         <f>SUM(G58:G63)</f>
         <v>0</v>
       </c>
     </row>
     <row r="65" spans="2:9" ht="30" customHeight="1" thickBot="1"/>
     <row r="66" spans="2:9" ht="60" customHeight="1">
-      <c r="B66" s="47" t="s">
+      <c r="B66" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="C66" s="48"/>
-      <c r="D66" s="48"/>
-      <c r="E66" s="48"/>
-      <c r="F66" s="48"/>
-      <c r="G66" s="48"/>
-      <c r="H66" s="48"/>
-      <c r="I66" s="49"/>
-    </row>
-    <row r="67" spans="2:9" ht="30" customHeight="1">
-      <c r="B67" s="14" t="s">
+      <c r="C66" s="19"/>
+      <c r="D66" s="19"/>
+      <c r="E66" s="19"/>
+      <c r="F66" s="19"/>
+      <c r="G66" s="19"/>
+      <c r="H66" s="19"/>
+      <c r="I66" s="20"/>
+    </row>
+    <row r="67" spans="2:9" ht="30" customHeight="1" thickBot="1">
+      <c r="B67" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="C67" s="42" t="s">
+      <c r="C67" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="D67" s="42"/>
-      <c r="E67" s="42"/>
-      <c r="F67" s="42"/>
+      <c r="D67" s="21"/>
+      <c r="E67" s="21"/>
+      <c r="F67" s="21"/>
       <c r="G67" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H67" s="42" t="s">
+      <c r="H67" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="I67" s="43"/>
-    </row>
-    <row r="68" spans="2:9" ht="30" customHeight="1">
-      <c r="B68" s="11"/>
-      <c r="C68" s="34"/>
-      <c r="D68" s="34"/>
-      <c r="E68" s="34"/>
-      <c r="F68" s="34"/>
+      <c r="I67" s="22"/>
+    </row>
+    <row r="68" spans="2:9" ht="30" customHeight="1" thickTop="1" thickBot="1">
+      <c r="B68" s="48"/>
+      <c r="C68" s="45"/>
+      <c r="D68" s="14"/>
+      <c r="E68" s="14"/>
+      <c r="F68" s="14"/>
       <c r="G68" s="1"/>
-      <c r="H68" s="34"/>
-      <c r="I68" s="44"/>
-    </row>
-    <row r="69" spans="2:9" ht="30" customHeight="1">
-      <c r="B69" s="11"/>
-      <c r="C69" s="34"/>
-      <c r="D69" s="34"/>
-      <c r="E69" s="34"/>
-      <c r="F69" s="34"/>
+      <c r="H68" s="14"/>
+      <c r="I68" s="15"/>
+    </row>
+    <row r="69" spans="2:9" ht="30" customHeight="1" thickTop="1" thickBot="1">
+      <c r="B69" s="48"/>
+      <c r="C69" s="45"/>
+      <c r="D69" s="14"/>
+      <c r="E69" s="14"/>
+      <c r="F69" s="14"/>
       <c r="G69" s="1"/>
-      <c r="H69" s="34"/>
-      <c r="I69" s="44"/>
-    </row>
-    <row r="70" spans="2:9" ht="30" customHeight="1">
-      <c r="B70" s="11"/>
-      <c r="C70" s="34"/>
-      <c r="D70" s="34"/>
-      <c r="E70" s="34"/>
-      <c r="F70" s="34"/>
+      <c r="H69" s="14"/>
+      <c r="I69" s="15"/>
+    </row>
+    <row r="70" spans="2:9" ht="30" customHeight="1" thickTop="1" thickBot="1">
+      <c r="B70" s="48"/>
+      <c r="C70" s="45"/>
+      <c r="D70" s="14"/>
+      <c r="E70" s="14"/>
+      <c r="F70" s="14"/>
       <c r="G70" s="1"/>
-      <c r="H70" s="34"/>
-      <c r="I70" s="44"/>
-    </row>
-    <row r="71" spans="2:9" ht="30" customHeight="1">
-      <c r="B71" s="11"/>
-      <c r="C71" s="34"/>
-      <c r="D71" s="34"/>
-      <c r="E71" s="34"/>
-      <c r="F71" s="34"/>
+      <c r="H70" s="14"/>
+      <c r="I70" s="15"/>
+    </row>
+    <row r="71" spans="2:9" ht="30" customHeight="1" thickTop="1" thickBot="1">
+      <c r="B71" s="48"/>
+      <c r="C71" s="45"/>
+      <c r="D71" s="14"/>
+      <c r="E71" s="14"/>
+      <c r="F71" s="14"/>
       <c r="G71" s="1"/>
-      <c r="H71" s="34"/>
-      <c r="I71" s="44"/>
-    </row>
-    <row r="72" spans="2:9" ht="30" customHeight="1">
-      <c r="B72" s="11"/>
-      <c r="C72" s="34"/>
-      <c r="D72" s="34"/>
-      <c r="E72" s="34"/>
-      <c r="F72" s="34"/>
+      <c r="H71" s="14"/>
+      <c r="I71" s="15"/>
+    </row>
+    <row r="72" spans="2:9" ht="30" customHeight="1" thickTop="1" thickBot="1">
+      <c r="B72" s="48"/>
+      <c r="C72" s="45"/>
+      <c r="D72" s="14"/>
+      <c r="E72" s="14"/>
+      <c r="F72" s="14"/>
       <c r="G72" s="1"/>
-      <c r="H72" s="34"/>
-      <c r="I72" s="44"/>
-    </row>
-    <row r="73" spans="2:9" ht="30" customHeight="1" thickBot="1">
-      <c r="B73" s="5"/>
-      <c r="C73" s="45"/>
-      <c r="D73" s="45"/>
-      <c r="E73" s="45"/>
-      <c r="F73" s="45"/>
+      <c r="H72" s="14"/>
+      <c r="I72" s="15"/>
+    </row>
+    <row r="73" spans="2:9" ht="30" customHeight="1" thickTop="1" thickBot="1">
+      <c r="B73" s="48"/>
+      <c r="C73" s="46"/>
+      <c r="D73" s="16"/>
+      <c r="E73" s="16"/>
+      <c r="F73" s="16"/>
       <c r="G73" s="2"/>
-      <c r="H73" s="45"/>
-      <c r="I73" s="46"/>
-    </row>
-    <row r="74" spans="2:9" ht="30" customHeight="1" thickBot="1">
-      <c r="F74" s="13" t="s">
+      <c r="H73" s="16"/>
+      <c r="I73" s="17"/>
+    </row>
+    <row r="74" spans="2:9" ht="30" customHeight="1" thickTop="1" thickBot="1">
+      <c r="F74" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="G74" s="12">
+      <c r="G74" s="10">
         <f>SUM(G68:G73)</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="100">
-    <mergeCell ref="C72:F72"/>
-    <mergeCell ref="H72:I72"/>
-    <mergeCell ref="C73:F73"/>
-    <mergeCell ref="H73:I73"/>
-    <mergeCell ref="C69:F69"/>
-    <mergeCell ref="H69:I69"/>
-    <mergeCell ref="C70:F70"/>
-    <mergeCell ref="H70:I70"/>
-    <mergeCell ref="C71:F71"/>
-    <mergeCell ref="H71:I71"/>
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="D4:I4"/>
+    <mergeCell ref="D5:I5"/>
+    <mergeCell ref="D6:I6"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="C20:F20"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B14:I14"/>
+    <mergeCell ref="B11:I11"/>
+    <mergeCell ref="B16:I16"/>
+    <mergeCell ref="C17:F17"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="C18:F18"/>
+    <mergeCell ref="C19:F19"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="C29:F29"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="C21:F21"/>
+    <mergeCell ref="C22:F22"/>
+    <mergeCell ref="C23:F23"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="B26:I26"/>
+    <mergeCell ref="C27:F27"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="C28:F28"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="C38:F38"/>
+    <mergeCell ref="H38:I38"/>
+    <mergeCell ref="C30:F30"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="C31:F31"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="C32:F32"/>
+    <mergeCell ref="H32:I32"/>
+    <mergeCell ref="C33:F33"/>
+    <mergeCell ref="H33:I33"/>
+    <mergeCell ref="B36:I36"/>
+    <mergeCell ref="C37:F37"/>
+    <mergeCell ref="H37:I37"/>
+    <mergeCell ref="C47:F47"/>
+    <mergeCell ref="H47:I47"/>
+    <mergeCell ref="C39:F39"/>
+    <mergeCell ref="H39:I39"/>
+    <mergeCell ref="C40:F40"/>
+    <mergeCell ref="H40:I40"/>
+    <mergeCell ref="C41:F41"/>
+    <mergeCell ref="H41:I41"/>
+    <mergeCell ref="C42:F42"/>
+    <mergeCell ref="H42:I42"/>
+    <mergeCell ref="C43:F43"/>
+    <mergeCell ref="H43:I43"/>
+    <mergeCell ref="B46:I46"/>
+    <mergeCell ref="C48:F48"/>
+    <mergeCell ref="H48:I48"/>
+    <mergeCell ref="C49:F49"/>
+    <mergeCell ref="H49:I49"/>
+    <mergeCell ref="C50:F50"/>
+    <mergeCell ref="H50:I50"/>
+    <mergeCell ref="C59:F59"/>
+    <mergeCell ref="H59:I59"/>
+    <mergeCell ref="C51:F51"/>
+    <mergeCell ref="H51:I51"/>
+    <mergeCell ref="C52:F52"/>
+    <mergeCell ref="H52:I52"/>
+    <mergeCell ref="C53:F53"/>
+    <mergeCell ref="H53:I53"/>
+    <mergeCell ref="B56:I56"/>
+    <mergeCell ref="C57:F57"/>
+    <mergeCell ref="H57:I57"/>
+    <mergeCell ref="C58:F58"/>
+    <mergeCell ref="H58:I58"/>
     <mergeCell ref="C68:F68"/>
     <mergeCell ref="H68:I68"/>
     <mergeCell ref="C60:F60"/>
@@ -2231,83 +2273,16 @@
     <mergeCell ref="B66:I66"/>
     <mergeCell ref="C67:F67"/>
     <mergeCell ref="H67:I67"/>
-    <mergeCell ref="C59:F59"/>
-    <mergeCell ref="H59:I59"/>
-    <mergeCell ref="C51:F51"/>
-    <mergeCell ref="H51:I51"/>
-    <mergeCell ref="C52:F52"/>
-    <mergeCell ref="H52:I52"/>
-    <mergeCell ref="C53:F53"/>
-    <mergeCell ref="H53:I53"/>
-    <mergeCell ref="B56:I56"/>
-    <mergeCell ref="C57:F57"/>
-    <mergeCell ref="H57:I57"/>
-    <mergeCell ref="C58:F58"/>
-    <mergeCell ref="H58:I58"/>
-    <mergeCell ref="C48:F48"/>
-    <mergeCell ref="H48:I48"/>
-    <mergeCell ref="C49:F49"/>
-    <mergeCell ref="H49:I49"/>
-    <mergeCell ref="C50:F50"/>
-    <mergeCell ref="H50:I50"/>
-    <mergeCell ref="C47:F47"/>
-    <mergeCell ref="H47:I47"/>
-    <mergeCell ref="C39:F39"/>
-    <mergeCell ref="H39:I39"/>
-    <mergeCell ref="C40:F40"/>
-    <mergeCell ref="H40:I40"/>
-    <mergeCell ref="C41:F41"/>
-    <mergeCell ref="H41:I41"/>
-    <mergeCell ref="C42:F42"/>
-    <mergeCell ref="H42:I42"/>
-    <mergeCell ref="C43:F43"/>
-    <mergeCell ref="H43:I43"/>
-    <mergeCell ref="B46:I46"/>
-    <mergeCell ref="C38:F38"/>
-    <mergeCell ref="H38:I38"/>
-    <mergeCell ref="C30:F30"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="C31:F31"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="C32:F32"/>
-    <mergeCell ref="H32:I32"/>
-    <mergeCell ref="C33:F33"/>
-    <mergeCell ref="H33:I33"/>
-    <mergeCell ref="B36:I36"/>
-    <mergeCell ref="C37:F37"/>
-    <mergeCell ref="H37:I37"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="C29:F29"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="C21:F21"/>
-    <mergeCell ref="C22:F22"/>
-    <mergeCell ref="C23:F23"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="B26:I26"/>
-    <mergeCell ref="C27:F27"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="C28:F28"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="C20:F20"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B14:I14"/>
-    <mergeCell ref="B11:I11"/>
-    <mergeCell ref="B16:I16"/>
-    <mergeCell ref="C17:F17"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="C18:F18"/>
-    <mergeCell ref="C19:F19"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="B2:I2"/>
-    <mergeCell ref="D4:I4"/>
-    <mergeCell ref="D5:I5"/>
-    <mergeCell ref="D6:I6"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="C72:F72"/>
+    <mergeCell ref="H72:I72"/>
+    <mergeCell ref="C73:F73"/>
+    <mergeCell ref="H73:I73"/>
+    <mergeCell ref="C69:F69"/>
+    <mergeCell ref="H69:I69"/>
+    <mergeCell ref="C70:F70"/>
+    <mergeCell ref="H70:I70"/>
+    <mergeCell ref="C71:F71"/>
+    <mergeCell ref="H71:I71"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="79" fitToHeight="4" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>